<commit_message>
End of the repairnator process
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -115,10 +115,10 @@
     <t>${event.attributes.toString().replaceAll(",", " ").replaceAll(bracketsRegex, "")}</t>
   </si>
   <si>
-    <t>${from.toString("YYYY.MM.dd HH:mm:ss")+" - "+to.toString("YYYY.MM.dd HH:mm:ss")}</t>
-  </si>
-  <si>
-    <t>${new("org.joda.time.DateTime", event.serverTime, timezone).toString("YYYY.MM.dd HH:mm:ss")}</t>
+    <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", event.serverTime, locale, timezone)}</t>
+  </si>
+  <si>
+    <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd HH:mm:ss", to, locale, timezone)}</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="7"/>
@@ -849,7 +849,7 @@
     </row>
     <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>11</v>

</xml_diff>